<commit_message>
add edited excel sheet
</commit_message>
<xml_diff>
--- a/cleaned_ldrgcr.xlsx
+++ b/cleaned_ldrgcr.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aditijoshi/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aditijoshi/Development/d2mr_transpose_to_quarto_aditij/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B6FFC67-A6BE-5D41-8FE5-C222DE8BC028}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDD1D1C4-99F8-A84E-BFFA-EF8487EE2EBD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14900" yWindow="720" windowWidth="14500" windowHeight="18400" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7660" yWindow="740" windowWidth="21740" windowHeight="16540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -182,7 +182,7 @@
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -493,10 +493,20 @@
   <dimension ref="A1:L100"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K1" sqref="K1"/>
+      <selection activeCell="M9" sqref="M9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="4" max="4" width="23.5" customWidth="1"/>
+    <col min="5" max="5" width="12" customWidth="1"/>
+    <col min="6" max="6" width="28.5" customWidth="1"/>
+    <col min="7" max="7" width="19.1640625" customWidth="1"/>
+    <col min="8" max="8" width="14.6640625" customWidth="1"/>
+    <col min="9" max="9" width="13.83203125" customWidth="1"/>
+    <col min="11" max="11" width="11.6640625" customWidth="1"/>
+    <col min="12" max="12" width="9.5" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">

</xml_diff>